<commit_message>
finished first iteration of battleManager
</commit_message>
<xml_diff>
--- a/Documentation_0.3_skill-trees.xlsx
+++ b/Documentation_0.3_skill-trees.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dylan\git\cs-2d-game\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dylan\git\monogame-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{241D2DF7-B4F6-415D-9969-38AEC5E86350}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDECA564-1227-47F5-A53E-8CD1AE7B8D36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8520" yWindow="2430" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5325" yWindow="1410" windowWidth="25650" windowHeight="15660" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Unit Overview" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1928" uniqueCount="901">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1946" uniqueCount="919">
   <si>
     <t>physical</t>
   </si>
@@ -2740,13 +2740,67 @@
   </si>
   <si>
     <t>Poison: Target takes damage = 15% of unit's Focus.</t>
+  </si>
+  <si>
+    <t>New Modifiers</t>
+  </si>
+  <si>
+    <t>8/16</t>
+  </si>
+  <si>
+    <t>8/15</t>
+  </si>
+  <si>
+    <t>8/14</t>
+  </si>
+  <si>
+    <t>8/13</t>
+  </si>
+  <si>
+    <t>8/12</t>
+  </si>
+  <si>
+    <t>8/11</t>
+  </si>
+  <si>
+    <t>8/9</t>
+  </si>
+  <si>
+    <t>8/8</t>
+  </si>
+  <si>
+    <t>8/10</t>
+  </si>
+  <si>
+    <t>16/8</t>
+  </si>
+  <si>
+    <t>15/8</t>
+  </si>
+  <si>
+    <t>14/8</t>
+  </si>
+  <si>
+    <t>13/8</t>
+  </si>
+  <si>
+    <t>12/8</t>
+  </si>
+  <si>
+    <t>11/8</t>
+  </si>
+  <si>
+    <t>10/8</t>
+  </si>
+  <si>
+    <t>9/8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2810,6 +2864,12 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="21">
@@ -3763,8 +3823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:H96"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:A19"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="I66" sqref="I66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4328,7 +4388,7 @@
   <dimension ref="A1:R128"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="M48" sqref="M48"/>
     </sheetView>
   </sheetViews>
@@ -9017,8 +9077,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:G109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R58" sqref="R58"/>
+    <sheetView topLeftCell="A76" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F100" sqref="F100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9606,7 +9666,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>729</v>
       </c>
@@ -9615,7 +9675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>730</v>
       </c>
@@ -9624,7 +9684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>731</v>
       </c>
@@ -9633,7 +9693,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>732</v>
       </c>
@@ -9642,7 +9702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>733</v>
       </c>
@@ -9651,7 +9711,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>816</v>
       </c>
@@ -9660,12 +9720,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>851</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E88" s="1" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="16">
         <v>-10</v>
       </c>
@@ -9676,8 +9739,9 @@
         <f>2/8</f>
         <v>0.25</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F89" s="37"/>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="16">
         <v>-9</v>
       </c>
@@ -9688,8 +9752,9 @@
         <f>1/3.75</f>
         <v>0.26666666666666666</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F90" s="37"/>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>-8</v>
       </c>
@@ -9700,8 +9765,14 @@
         <f>1/3.5</f>
         <v>0.2857142857142857</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E91" s="78" t="s">
+        <v>902</v>
+      </c>
+      <c r="F91" s="37">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>-7</v>
       </c>
@@ -9712,8 +9783,14 @@
         <f>1/3.25</f>
         <v>0.30769230769230771</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E92" s="78" t="s">
+        <v>903</v>
+      </c>
+      <c r="F92" s="37">
+        <v>0.5333</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>-6</v>
       </c>
@@ -9724,8 +9801,14 @@
         <f>2/6</f>
         <v>0.33333333333333331</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E93" s="78" t="s">
+        <v>904</v>
+      </c>
+      <c r="F93" s="37">
+        <v>0.57140000000000002</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>-5</v>
       </c>
@@ -9736,8 +9819,14 @@
         <f>1/2.75</f>
         <v>0.36363636363636365</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E94" s="78" t="s">
+        <v>905</v>
+      </c>
+      <c r="F94" s="37">
+        <v>0.61539999999999995</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>-4</v>
       </c>
@@ -9748,8 +9837,14 @@
         <f>1/2.5</f>
         <v>0.4</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E95" s="78" t="s">
+        <v>906</v>
+      </c>
+      <c r="F95" s="37">
+        <v>0.66659999999999997</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>-3</v>
       </c>
@@ -9760,8 +9855,14 @@
         <f>1/2.25</f>
         <v>0.44444444444444442</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E96" s="78" t="s">
+        <v>907</v>
+      </c>
+      <c r="F96" s="37">
+        <v>0.72719999999999996</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>-2</v>
       </c>
@@ -9772,8 +9873,14 @@
         <f>1/2</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E97" s="78" t="s">
+        <v>910</v>
+      </c>
+      <c r="F97" s="37">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>-1</v>
       </c>
@@ -9784,8 +9891,14 @@
         <f>1/1.5</f>
         <v>0.66666666666666663</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E98" s="78" t="s">
+        <v>908</v>
+      </c>
+      <c r="F98" s="37">
+        <v>0.88880000000000003</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>0</v>
       </c>
@@ -9795,8 +9908,14 @@
       <c r="C99" s="37">
         <v>1</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E99" s="78" t="s">
+        <v>909</v>
+      </c>
+      <c r="F99" s="37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>1</v>
       </c>
@@ -9806,8 +9925,14 @@
       <c r="C100" s="37">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E100" s="78" t="s">
+        <v>918</v>
+      </c>
+      <c r="F100" s="37">
+        <v>1.125</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>2</v>
       </c>
@@ -9817,8 +9942,14 @@
       <c r="C101" s="37">
         <v>2</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E101" s="78" t="s">
+        <v>917</v>
+      </c>
+      <c r="F101" s="37">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>3</v>
       </c>
@@ -9828,8 +9959,14 @@
       <c r="C102" s="37">
         <v>2.25</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E102" s="78" t="s">
+        <v>916</v>
+      </c>
+      <c r="F102" s="37">
+        <v>1.375</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>4</v>
       </c>
@@ -9839,8 +9976,14 @@
       <c r="C103" s="37">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E103" s="78" t="s">
+        <v>915</v>
+      </c>
+      <c r="F103" s="37">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>5</v>
       </c>
@@ -9850,8 +9993,14 @@
       <c r="C104" s="37">
         <v>2.75</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E104" s="78" t="s">
+        <v>914</v>
+      </c>
+      <c r="F104" s="37">
+        <v>1.625</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>6</v>
       </c>
@@ -9861,8 +10010,14 @@
       <c r="C105" s="37">
         <v>3</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E105" s="78" t="s">
+        <v>913</v>
+      </c>
+      <c r="F105" s="37">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>7</v>
       </c>
@@ -9872,8 +10027,14 @@
       <c r="C106" s="37">
         <v>3.25</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E106" s="78" t="s">
+        <v>912</v>
+      </c>
+      <c r="F106" s="37">
+        <v>1.875</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>8</v>
       </c>
@@ -9883,8 +10044,14 @@
       <c r="C107" s="37">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E107" s="78" t="s">
+        <v>911</v>
+      </c>
+      <c r="F107" s="37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>9</v>
       </c>
@@ -9894,8 +10061,10 @@
       <c r="C108" s="37">
         <v>3.75</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E108" s="78"/>
+      <c r="F108" s="37"/>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>10</v>
       </c>
@@ -9905,8 +10074,11 @@
       <c r="C109" s="37">
         <v>4</v>
       </c>
+      <c r="E109" s="78"/>
+      <c r="F109" s="37"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -9916,9 +10088,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:N194"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D173" sqref="D173"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>